<commit_message>
Final ver 1.0 without logging
</commit_message>
<xml_diff>
--- a/ZMAT_LIST.xlsx
+++ b/ZMAT_LIST.xlsx
@@ -534,7 +534,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -846,13 +846,13 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="9">
-        <v>3000009096</v>
+        <v>3000009097</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -860,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -871,13 +871,13 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="9">
-        <v>3000009097</v>
+        <v>3000009096</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -885,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -994,7 +994,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" s="6" customFormat="1">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1">
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>11</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" s="6" customFormat="1">
       <c r="A22" s="1">
         <v>12</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1">
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
         <v>15</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" s="6" customFormat="1">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1330,12 +1330,6 @@
       <c r="G30" s="2">
         <v>25</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" s="6" customFormat="1">
       <c r="A31" s="1">
@@ -1383,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -1443,6 +1437,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x010100C1F3A0CDEB9FC747AB83298D37E80C9D" ma:contentTypeVersion="6" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="0fdd988da03b41f8d2cfdb2f64bef85d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f79893ca-c046-45dd-bbb7-92a4bddb12a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2c0d965aa1805eaf111d4f42478cbbe" ns2:_="">
     <xsd:import namespace="f79893ca-c046-45dd-bbb7-92a4bddb12a7"/>
@@ -1607,21 +1616,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F53A843-70D7-43D8-A044-01251CA89430}">
   <ds:schemaRefs>
@@ -1631,19 +1625,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C5EEAC4-D335-47A0-B536-F07660F6510D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ECD3B30-B132-4A56-A39E-13C12E1E8864}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f79893ca-c046-45dd-bbb7-92a4bddb12a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1667,9 +1651,19 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ECD3B30-B132-4A56-A39E-13C12E1E8864}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C5EEAC4-D335-47A0-B536-F07660F6510D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f79893ca-c046-45dd-bbb7-92a4bddb12a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>